<commit_message>
add api_operations and additional argument checks
- now expect conceptId and concept arguments to be length 1
- api_browser_concept_parents
- api_concept_descendants
- api_concept_descriptions
- api_browser_concept_descriptions
- api_descriptions_semantic_tags
</commit_message>
<xml_diff>
--- a/data-raw/api_operations_backlog.xlsx
+++ b/data-raw/api_operations_backlog.xlsx
@@ -562,10 +562,10 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.35"/>
@@ -617,8 +617,8 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G2" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -642,8 +642,8 @@
         <v>14</v>
       </c>
       <c r="F3" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -667,8 +667,8 @@
         <v>17</v>
       </c>
       <c r="F4" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G4" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -692,8 +692,8 @@
         <v>20</v>
       </c>
       <c r="F5" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G5" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -717,8 +717,8 @@
         <v>23</v>
       </c>
       <c r="F6" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -742,8 +742,8 @@
         <v>26</v>
       </c>
       <c r="F7" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -767,8 +767,8 @@
         <v>29</v>
       </c>
       <c r="F8" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -792,8 +792,8 @@
         <v>32</v>
       </c>
       <c r="F9" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -870,8 +870,8 @@
         <v>42</v>
       </c>
       <c r="F12" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -895,8 +895,8 @@
         <v>45</v>
       </c>
       <c r="F13" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G13" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -920,8 +920,8 @@
         <v>48</v>
       </c>
       <c r="F14" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G14" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -945,8 +945,8 @@
         <v>51</v>
       </c>
       <c r="F15" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G15" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -970,8 +970,8 @@
         <v>54</v>
       </c>
       <c r="F16" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G16" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -1395,8 +1395,8 @@
         <v>105</v>
       </c>
       <c r="F33" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="G33" s="2" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>

<commit_message>
add concepts_ascendants() wrapper function
</commit_message>
<xml_diff>
--- a/data-raw/api_operations_backlog.xlsx
+++ b/data-raw/api_operations_backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27720" windowHeight="12450" tabRatio="500"/>
+    <workbookView windowWidth="19200" windowHeight="12015" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
     <t>api_concepts</t>
   </si>
   <si>
-    <t>concepts_find; concepts_descendants</t>
+    <t>concepts_find; concepts_ascendants; concepts_descendants</t>
   </si>
   <si>
     <t>/{branch}/concepts/{conceptId}</t>
@@ -496,10 +496,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -508,17 +508,18 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -531,9 +532,24 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -545,16 +561,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -577,9 +585,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,7 +599,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -608,15 +614,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,31 +651,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -668,13 +668,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,163 +842,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,17 +862,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -896,21 +896,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -921,17 +906,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,157 +927,183 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1445,8 +1445,8 @@
   <sheetPr/>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="12.75" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
correct API operations spreadsheet.   /browser/{branch}/concepts is not implemented. /browser/{branch}/concepts/{conceptId} is implemented
</commit_message>
<xml_diff>
--- a/data-raw/api_operations_backlog.xlsx
+++ b/data-raw/api_operations_backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sejjpfd\AppData\Local\0_git_repos\04_snomed\snomedizer\data-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F728E-5C76-4C26-9062-B510C968C4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="12015" tabRatio="500"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$46</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -493,367 +511,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -861,318 +544,37 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
         <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <family val="2"/>
         <charset val="1"/>
-        <family val="2"/>
+        <scheme val="none"/>
       </font>
     </dxf>
   </dxfs>
@@ -1180,6 +582,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1303,7 +708,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1327,9 +732,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1353,7 +758,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1406,7 +811,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="true">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1431,35 +836,35 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="false"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="12.75" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.57142857142857" customWidth="true"/>
-    <col min="2" max="2" width="7.28571428571429" customWidth="true"/>
-    <col min="3" max="3" width="49.8571428571429" customWidth="true"/>
-    <col min="4" max="4" width="71.4285714285714" customWidth="true"/>
-    <col min="5" max="5" width="26" customWidth="true"/>
-    <col min="8" max="8" width="19.2571428571429" customWidth="true"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="71.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1485,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
@@ -1506,11 +911,11 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="b">
-        <f t="shared" ref="G2:G8" si="1">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <f t="shared" ref="F2:G8" si="1">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1535,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>11</v>
       </c>
@@ -1560,7 +965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>15</v>
       </c>
@@ -1573,19 +978,17 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
+      <c r="E5" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="3" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>17</v>
       </c>
@@ -1599,10 +1002,10 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G6" s="3" t="b">
@@ -1610,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>18</v>
       </c>
@@ -1635,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>19</v>
       </c>
@@ -1660,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1680,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -1705,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21</v>
       </c>
@@ -1733,7 +1136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22</v>
       </c>
@@ -1758,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>24</v>
       </c>
@@ -1783,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1808,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>29</v>
       </c>
@@ -1833,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
@@ -1861,7 +1264,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>43</v>
       </c>
@@ -1886,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1911,7 +1314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1936,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1961,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1986,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2011,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2036,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2061,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2086,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>12</v>
       </c>
@@ -2111,7 +1514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
@@ -2136,7 +1539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
@@ -2161,7 +1564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>16</v>
       </c>
@@ -2186,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
@@ -2211,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>26</v>
       </c>
@@ -2236,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>27</v>
       </c>
@@ -2261,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>28</v>
       </c>
@@ -2286,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2311,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2336,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2361,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -2383,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2408,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2433,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>36</v>
       </c>
@@ -2458,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2483,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2511,7 +1914,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>39</v>
       </c>
@@ -2536,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2561,7 +1964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>41</v>
       </c>
@@ -2586,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>42</v>
       </c>
@@ -2611,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>147</v>
       </c>
@@ -2633,7 +2036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:7">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>147</v>
       </c>
@@ -2655,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:7">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>8</v>
       </c>
@@ -2677,7 +2080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:7">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>8</v>
       </c>
@@ -2699,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:7">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>8</v>
       </c>
@@ -2722,17 +2125,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G46">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E51">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
update api backlog #31 and changelog
</commit_message>
<xml_diff>
--- a/data-raw/api_operations_backlog.xlsx
+++ b/data-raw/api_operations_backlog.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sejjpfd\AppData\Local\0_git_repos\04_snomed\snomedizer\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991F728E-5C76-4C26-9062-B510C968C4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5510B3AA-C73E-4131-921F-6E07D6A65D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="159">
   <si>
     <t>pos</t>
   </si>
@@ -55,9 +55,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>pAMR requirement</t>
-  </si>
-  <si>
     <t>wrapper</t>
   </si>
   <si>
@@ -506,6 +503,15 @@
   </si>
   <si>
     <t xml:space="preserve">/actuator/info </t>
+  </si>
+  <si>
+    <t>/validation-maintenance/semantic-tags</t>
+  </si>
+  <si>
+    <t>Retrieve all semantic tags.</t>
+  </si>
+  <si>
+    <t>api_semantic_tags</t>
   </si>
 </sst>
 </file>
@@ -848,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -861,10 +867,10 @@
     <col min="3" max="3" width="49.85546875" customWidth="1"/>
     <col min="4" max="4" width="71.42578125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,1254 +889,1064 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="F2" s="3" t="b">
         <f t="shared" ref="F2:F8" si="0">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="b">
-        <f t="shared" ref="F2:G8" si="1">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="3" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F4" s="3" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G4" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F6" si="1">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="3" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F8" s="3" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="F9" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="F10" s="3" t="b">
         <f t="shared" ref="F10:F17" si="2">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G10" s="3" t="b">
-        <f t="shared" ref="G10:G17" si="3">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="F11" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G11" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F12" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G12" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
         <v>43</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="F13" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G13" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F14" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G14" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G15" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="F16" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G16" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
         <v>56</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="F17" s="3" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G17" s="3" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F18" s="3" t="b">
-        <f t="shared" ref="F18:F33" si="4">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="3" t="b">
-        <f t="shared" ref="G18:G51" si="5">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F18:F33" si="3">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
         <v>62</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F19" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
         <v>65</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="F20" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>68</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="F21" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="F22" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="3" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F24" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
         <v>80</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F25" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" t="s">
         <v>83</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="F26" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" t="s">
         <v>86</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F27" s="3" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G27" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" t="s">
         <v>89</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F28" s="3" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="G28" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" t="s">
         <v>92</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="F29" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" t="s">
         <v>95</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="F30" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" t="s">
         <v>98</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="F31" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
         <v>101</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="F32" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
         <v>104</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="F33" s="3" t="b">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" t="s">
         <v>107</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F34" s="3" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G34" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" t="s">
         <v>110</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="F35" s="3" t="b">
-        <f t="shared" ref="F35:F51" si="6">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F35:F52" si="4">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" t="s">
         <v>113</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G36" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>116</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="F37" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G37" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" t="s">
         <v>119</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="F38" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39" t="s">
         <v>122</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>124</v>
-      </c>
       <c r="F39" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" t="s">
         <v>125</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="F40" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
         <v>128</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="F41" s="3" t="b">
-        <f t="shared" ref="F41:F45" si="7">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G41" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ref="F41:F45" si="5">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C42" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" t="s">
         <v>131</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="3" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
         <v>133</v>
       </c>
-      <c r="F42" s="3" t="b">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G42" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H42" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
+        <v>134</v>
+      </c>
+      <c r="D43" t="s">
         <v>135</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="F43" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G43" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
         <v>138</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="F44" s="3" t="b">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G44" s="3" t="b">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" t="s">
         <v>141</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="3" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>156</v>
+      </c>
+      <c r="D46" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
         <v>143</v>
       </c>
-      <c r="F45" s="3" t="b">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G45" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>42</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D47" t="s">
         <v>144</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E47" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F47" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>146</v>
       </c>
-      <c r="F46" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
+      <c r="C48" t="s">
         <v>147</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D48" t="s">
         <v>148</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E48" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F48" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>150</v>
       </c>
-      <c r="F47" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G47" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D49" t="s">
         <v>151</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E49" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>152</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F48" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D50" t="s">
         <v>153</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F50" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
         <v>154</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F49" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G49" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="D51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51" s="3" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
         <v>155</v>
       </c>
-      <c r="D50" t="s">
-        <v>154</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F50" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G50" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" t="s">
-        <v>156</v>
-      </c>
-      <c r="D51" t="s">
-        <v>154</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" s="3" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G51" s="3" t="b">
-        <f t="shared" si="5"/>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F52" s="3" t="b">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="E2:E48">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  <autoFilter ref="A1:F52" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="E50:E52">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E51">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="E2:E49">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>